<commit_message>
Cleaned up Jupyter notebook and added a chart of LinearSVM model
</commit_message>
<xml_diff>
--- a/ppt/chart.xlsx
+++ b/ppt/chart.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hasanhaq/metis_hasan/projects/03-flows/ppt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hasanhaq/malware_metis/ppt/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="460" windowWidth="19260" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="9120" yWindow="2140" windowWidth="19260" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chart" sheetId="1" r:id="rId1"/>
+    <sheet name="packets" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Random Forests</t>
   </si>
@@ -52,6 +53,51 @@
   <si>
     <t>LinearSVC</t>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Src Port</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Dst Port</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Total Bytes</t>
+  </si>
+  <si>
+    <t>Num. Packets</t>
+  </si>
+  <si>
+    <t>Duration (Secs)</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
+  </si>
+  <si>
+    <t>123.45.67.89</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>&lt;-&gt;</t>
+  </si>
+  <si>
+    <t>184.50.238.145</t>
+  </si>
+  <si>
+    <t>184.50.238.187</t>
+  </si>
 </sst>
 </file>
 
@@ -71,15 +117,33 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -87,13 +151,304 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,11 +681,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="588322576"/>
-        <c:axId val="588324352"/>
+        <c:axId val="252687888"/>
+        <c:axId val="253244208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="588322576"/>
+        <c:axId val="252687888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -370,7 +725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588324352"/>
+        <c:crossAx val="253244208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -378,7 +733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588324352"/>
+        <c:axId val="253244208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +743,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588322576"/>
+        <c:crossAx val="252687888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -646,11 +1001,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="519465600"/>
-        <c:axId val="519467920"/>
+        <c:axId val="253255760"/>
+        <c:axId val="253258512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="519465600"/>
+        <c:axId val="253255760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,7 +1045,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="519467920"/>
+        <c:crossAx val="253258512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -698,7 +1053,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519467920"/>
+        <c:axId val="253258512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,7 +1063,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="519465600"/>
+        <c:crossAx val="253255760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -904,7 +1259,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -963,11 +1317,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="588346848"/>
-        <c:axId val="519472720"/>
+        <c:axId val="253279040"/>
+        <c:axId val="253281792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="588346848"/>
+        <c:axId val="253279040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,7 +1361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="519472720"/>
+        <c:crossAx val="253281792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1015,7 +1369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="519472720"/>
+        <c:axId val="253281792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,7 +1378,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588346848"/>
+        <c:crossAx val="253279040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1291,11 +1645,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="588358480"/>
-        <c:axId val="588360800"/>
+        <c:axId val="253302464"/>
+        <c:axId val="253305216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="588358480"/>
+        <c:axId val="253302464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1335,7 +1689,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588360800"/>
+        <c:crossAx val="253305216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1343,7 +1697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588360800"/>
+        <c:axId val="253305216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,7 +1706,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588358480"/>
+        <c:crossAx val="253302464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3966,7 +4320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -4115,4 +4469,277 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="8">
+        <v>42810.631053240744</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="9">
+        <v>54546</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="10">
+        <v>42810.631053240744</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="11">
+        <v>22</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="11">
+        <v>54546</v>
+      </c>
+      <c r="G4" s="12">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="10">
+        <v>42810.631168981483</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="11">
+        <v>22</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11">
+        <v>54546</v>
+      </c>
+      <c r="G5" s="12">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
+        <v>42810.631226851852</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="20">
+        <v>54546</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="20">
+        <v>22</v>
+      </c>
+      <c r="G6" s="18">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="13">
+        <v>42810.641076388885</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="14">
+        <v>55725</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="14">
+        <v>80</v>
+      </c>
+      <c r="G7" s="15">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="16">
+        <v>42810.641076388885</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3">
+        <v>80</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3">
+        <v>55715</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="17">
+        <v>42810.641111111108</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>55717</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="5">
+        <v>80</v>
+      </c>
+      <c r="G9" s="6">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="21">
+        <v>15</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9">
+        <v>54546</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9">
+        <v>22</v>
+      </c>
+      <c r="G12" s="9">
+        <f>SUM(G3:G6)</f>
+        <v>828</v>
+      </c>
+      <c r="H12" s="9">
+        <f>COUNT(G3:G6)</f>
+        <v>4</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5">
+        <v>55717</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5">
+        <v>80</v>
+      </c>
+      <c r="G13" s="5">
+        <f>SUM(G7:G9)</f>
+        <v>2631</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G12:G13 H12" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up some comments
</commit_message>
<xml_diff>
--- a/ppt/chart.xlsx
+++ b/ppt/chart.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hasanhaq/malware_metis/ppt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hasanhaq/malware_classify/ppt/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="2140" windowWidth="19260" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1520" yWindow="480" windowWidth="19260" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="chart" sheetId="1" r:id="rId1"/>
     <sheet name="packets" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Random Forests</t>
   </si>
@@ -98,12 +99,87 @@
   <si>
     <t>184.50.238.187</t>
   </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>Dur</t>
+  </si>
+  <si>
+    <t>Proto</t>
+  </si>
+  <si>
+    <t>SrcAddr</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Dir</t>
+  </si>
+  <si>
+    <t>DstAddr</t>
+  </si>
+  <si>
+    <t>Dport</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>TotPkts</t>
+  </si>
+  <si>
+    <t>TotBytes</t>
+  </si>
+  <si>
+    <t>SrcBytes</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>203.253.8.233</t>
+  </si>
+  <si>
+    <t>147.32.84.229</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>81.47.154.13</t>
+  </si>
+  <si>
+    <t>RPA_PA</t>
+  </si>
+  <si>
+    <t>78.42.25.171</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>113.128.219.130</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +191,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -143,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -379,11 +471,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,8 +638,61 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="47" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="47" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="47" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,7 +751,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -610,7 +851,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -681,11 +921,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="252687888"/>
-        <c:axId val="253244208"/>
+        <c:axId val="887136640"/>
+        <c:axId val="887141088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252687888"/>
+        <c:axId val="887136640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +965,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253244208"/>
+        <c:crossAx val="887141088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -733,7 +973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253244208"/>
+        <c:axId val="887141088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +983,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252687888"/>
+        <c:crossAx val="887136640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -829,7 +1069,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -930,7 +1169,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1001,11 +1239,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="253255760"/>
-        <c:axId val="253258512"/>
+        <c:axId val="923612432"/>
+        <c:axId val="923615184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253255760"/>
+        <c:axId val="923612432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1283,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253258512"/>
+        <c:crossAx val="923615184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1053,7 +1291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253258512"/>
+        <c:axId val="923615184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,7 +1301,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="253255760"/>
+        <c:crossAx val="923612432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1317,11 +1555,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="253279040"/>
-        <c:axId val="253281792"/>
+        <c:axId val="923636144"/>
+        <c:axId val="923638896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253279040"/>
+        <c:axId val="923636144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1361,7 +1599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253281792"/>
+        <c:crossAx val="923638896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1369,7 +1607,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253281792"/>
+        <c:axId val="923638896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,7 +1616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="253279040"/>
+        <c:crossAx val="923636144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1574,7 +1812,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1645,11 +1882,11 @@
         </c:dLbls>
         <c:gapWidth val="96"/>
         <c:overlap val="14"/>
-        <c:axId val="253302464"/>
-        <c:axId val="253305216"/>
+        <c:axId val="887194144"/>
+        <c:axId val="887196192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253302464"/>
+        <c:axId val="887194144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1689,7 +1926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253305216"/>
+        <c:crossAx val="887196192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1697,7 +1934,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253305216"/>
+        <c:axId val="887196192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,7 +1943,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="253302464"/>
+        <c:crossAx val="887194144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4475,8 +4712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4742,4 +4979,243 @@
     <ignoredError sqref="G12:G13 H12" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="34">
+        <v>40766.409441215277</v>
+      </c>
+      <c r="C3" s="37">
+        <v>2069.9731449999999</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="28">
+        <v>30533</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="28">
+        <v>13363</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="28">
+        <v>3</v>
+      </c>
+      <c r="L3" s="28">
+        <v>197</v>
+      </c>
+      <c r="M3" s="28">
+        <v>123</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="35">
+        <v>40766.409441226853</v>
+      </c>
+      <c r="C4" s="38">
+        <v>895.98925799999995</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="23">
+        <v>49200</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="23">
+        <v>13363</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="23">
+        <v>70</v>
+      </c>
+      <c r="L4" s="23">
+        <v>7032</v>
+      </c>
+      <c r="M4" s="23">
+        <v>4501</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="35">
+        <v>40766.409441226853</v>
+      </c>
+      <c r="C5" s="38">
+        <v>1.2E-4</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="23">
+        <v>13363</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="23">
+        <v>42988</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="23">
+        <v>3</v>
+      </c>
+      <c r="L5" s="23">
+        <v>2858</v>
+      </c>
+      <c r="M5" s="23">
+        <v>2858</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36">
+        <v>40766.409441238429</v>
+      </c>
+      <c r="C6" s="39">
+        <v>3561.9272460000002</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="26">
+        <v>13363</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="26">
+        <v>59790</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="26">
+        <v>63</v>
+      </c>
+      <c r="L6" s="26">
+        <v>15770</v>
+      </c>
+      <c r="M6" s="26">
+        <v>13419</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>